<commit_message>
Update: addedd better figures. TODO: improve the figures.
</commit_message>
<xml_diff>
--- a/materials/conditions.xlsx
+++ b/materials/conditions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokumenty_Ania\eyetrackery\eyetracker\materials\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mikolaj/Desktop/eyetracker/materials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C2EC6E0-1419-44F6-BD25-FFDDA04BA2E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EEFD521-FF38-794E-8F6C-CAFCAA6DAB71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="conditions" sheetId="1" r:id="rId1"/>
@@ -55,9 +55,6 @@
     <t>png/smartwatch.png</t>
   </si>
   <si>
-    <t>png/smartband.png</t>
-  </si>
-  <si>
     <t>smartband</t>
   </si>
   <si>
@@ -71,10 +68,6 @@
   </si>
   <si>
     <t>cena: 249 zł</t>
-  </si>
-  <si>
-    <t>Ekran o przekątnej 15.6" i wysokiej rozdzielczości z matową powłoką ograniczającą odbijanie się promieni słonecznych. \n Dwurdzeniowy procesor i 8 GB pamięci RAM  pozwalającej na uruchomienie kilku aplikacji jednocześnie oraz granie w wymagające sprzętowo gry komputerowe, pojemność dysku SSD 256 GB.\n
-Ślad węglowy to 423 kg</t>
   </si>
   <si>
     <t>Praca na nim przebiega płynnie, ekran rzeczywiście ładnie odwzorowuje kolory. Polecam!\n
@@ -110,6 +103,14 @@
     <t>Bardzo dobry zakup. Wygląda jak smartwatch, estetycznie wykonany , posiada wielorakie funkcje, których szukałem. No i możliwości sparowania są na plus!\n
 Udany zakup. Spełnił wszystkie moje oczekiwania. Nawet na chudszej ręce dobrze się prezentuje. Zgrabny, czytelny, wygodny.\n
 Przyjazny środowisku :) . Do tego wygląda jak opaska, ale możliwości ma raczej smartwatcha. Dla mnie super!</t>
+  </si>
+  <si>
+    <t>Ekran o przekątnej 15.6" i wysokiej rozdzielczości z matową powłoką ograniczającą odbijanie się promieni słonecznych\n 
+Dwurdzeniowy procesor i 8 GB pamięci RAM  pozwalającej na uruchomienie kilku aplikacji jednocześnie oraz granie w wymagające sprzętowo gry komputerowe, pojemność dysku SSD 256 GB.\n
+Ślad węglowy to 423 kg</t>
+  </si>
+  <si>
+    <t>png/smartband2.png</t>
   </si>
 </sst>
 </file>
@@ -675,7 +676,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office 2013 — 2022">
   <a:themeElements>
     <a:clrScheme name="Pakiet Office">
       <a:dk1>
@@ -963,7 +964,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -973,18 +974,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="18.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1001,72 +1002,72 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="362.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="388" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="252" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="306" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="346.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="388" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="299.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="323" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s">
         <v>24</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add: better quality pictures. Update: scales. TODO: write out the scales to a file. better quality radio buttons and scales in general (add question about price to carbon questions).
</commit_message>
<xml_diff>
--- a/materials/conditions.xlsx
+++ b/materials/conditions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mikolaj/Desktop/eyetracker/materials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EEFD521-FF38-794E-8F6C-CAFCAA6DAB71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1923230-B6F0-5046-B568-9B952258180B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -110,7 +110,7 @@
 Ślad węglowy to 423 kg</t>
   </si>
   <si>
-    <t>png/smartband2.png</t>
+    <t>png/smartband.png</t>
   </si>
 </sst>
 </file>
@@ -676,7 +676,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office 2013 — 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
   <a:themeElements>
     <a:clrScheme name="Pakiet Office">
       <a:dk1>
@@ -964,7 +964,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -975,7 +975,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
TODO: Writing out data.
</commit_message>
<xml_diff>
--- a/materials/conditions.xlsx
+++ b/materials/conditions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mikolaj/Desktop/eyetracker/materials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1923230-B6F0-5046-B568-9B952258180B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{693580C7-3FBD-DB4C-B1D5-C385F790476D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -70,47 +70,47 @@
     <t>cena: 249 zł</t>
   </si>
   <si>
-    <t>Praca na nim przebiega płynnie, ekran rzeczywiście ładnie odwzorowuje kolory. Polecam!\n
-Ogólnie spoko, szybko przyzwyczaiłam się do klawiatury, wentylator chodzi na tyle cicho, że mi nie przeszkadza, bateria starcza na tyle, ile powinna. Bardzo fajny laptop.\n
+    <t>png/smartband.png</t>
+  </si>
+  <si>
+    <t>Ekran o przekątnej 15.6" i wysokiej rozdzielczości z matową powłoką ograniczającą odbijanie się promieni słonecznych. \n
+Dwurdzeniowy procesor i 8 GB pamięci RAM  pozwalającej na uruchomienie kilku aplikacji jednocześnie oraz granie w wymagające sprzętowo gry komputerowe, pojemność dysku SSD 256 GB. \n
+Ślad węglowy to 423 kg</t>
+  </si>
+  <si>
+    <t>Praca na nim przebiega płynnie, ekran rzeczywiście ładnie odwzorowuje kolory. Polecam! \n
+Ogólnie spoko, szybko przyzwyczaiłam się do klawiatury, wentylator chodzi na tyle cicho, że mi nie przeszkadza, bateria starcza na tyle, ile powinna. Bardzo fajny laptop. \n
 Urządzenie w całości z solidnego i trwałego tworzywa, firma stawia na zrównoważony rozwój :).</t>
   </si>
   <si>
-    <t>Posiada czytelny wyświetlacz o przekątnej 10,5 cala i dwa aparaty, tylny aparat pozwala nagrywać w Full HD.\n
-Akumulator o pojemności 7040 mAh z opcją szybkiego ładowania, 4 GB pamięci RAM pozwala obsługiwać kilka aplikacji naraz.\n
+    <t>Posiada czytelny wyświetlacz o przekątnej 10,5 cala i dwa aparaty, tylny aparat pozwala nagrywać w Full HD. \n
+Akumulator o pojemności 7040 mAh z opcją szybkiego ładowania, 4 GB pamięci RAM pozwala obsługiwać kilka aplikacji naraz. \n
 Ślad węglowy: 170 kg</t>
   </si>
   <si>
-    <t xml:space="preserve">Jestem zadowolona, jakość adekwatna do ceny , a nawet lepsza.\n
-Działa sprawnie, jest pojemny, nie grzeje się przesadnie. Kupiłem go dla córki, katuje go dziennie (gry, lekcje, bajki, etc). Daje radę. Polecam!\n
+    <t xml:space="preserve">Jestem zadowolona, jakość adekwatna do ceny , a nawet lepsza. \n
+Działa sprawnie, jest pojemny, nie grzeje się przesadnie. Kupiłem go dla córki, katuje go dziennie (gry, lekcje, bajki, etc). Daje radę. Polecam! \n
 Solidny, dobrze wykonany, przez pro-ekolofgiczną firmę. Dla mnie spełnia oczekiwania. </t>
   </si>
   <si>
-    <t>Pomógł mi zadbać o zdrowie, fajnie się z nim ćwiczy. Bateria mi trzymała raczej nieźle, a jestem na to wyczulona. Ogólnie Polecam. Jestem super zadowolona. (Idealnie współpracuje z moim smartfonem).\n
-Warty każdej złotówki. To zdecydowanie nie jest zabawka. Porządnie złożony, świetnie zaprojektowany. Spełnia oczekiwania w 100%, gorąco polecam.\n
-Super sprzęt. Zegarek i do sportu i do noszenia na co dzień. Do tego wykonany z troską o środowisko.</t>
-  </si>
-  <si>
-    <t>Bezprzewodowa łączność ze smartphonem (Android i iOS), automatyczne wykrywanie 3 trybów: bieżnia, bieganie lub spacery na świeżym powietrzu.\n
-Przy standardowym użytkowaniu  do 14 dni na jednym naładowaniu baterii - w trybie oszczędzania baterii maksymalnie do 20 dni.\n
-Ślad węglowy: 36 kg</t>
-  </si>
-  <si>
-    <t>Czytelny wyświetlacz 1.4”, bezprzewodowa łączność ze smartphonem (Android i iOS), asystent zdrowotny z funkcjami pomiaru ciśnienia i EKG, analizą składu ciała, zaawansowaną analiza snu i czujnikami aktywności fizycznej.\n
+    <t>Czytelny wyświetlacz 1.4”, bezprzewodowa łączność ze smartphonem (Android i iOS), asystent zdrowotny z funkcjami pomiaru ciśnienia i EKG, analizą składu ciała, zaawansowaną analiza snu i czujnikami aktywności fizycznej. \n
 Bateria pracuje do 40 godzin, można ją naładować od 0% w 1 godzinę i 48 minut, posiada 16 GB pamięci wewnętrznej. \n
 Ślad węglowy: 43 kg</t>
   </si>
   <si>
-    <t>Bardzo dobry zakup. Wygląda jak smartwatch, estetycznie wykonany , posiada wielorakie funkcje, których szukałem. No i możliwości sparowania są na plus!\n
-Udany zakup. Spełnił wszystkie moje oczekiwania. Nawet na chudszej ręce dobrze się prezentuje. Zgrabny, czytelny, wygodny.\n
+    <t>Pomógł mi zadbać o zdrowie, fajnie się z nim ćwiczy. Bateria mi trzymała raczej nieźle, a jestem na to wyczulona. Ogólnie Polecam. Jestem super zadowolona. (Idealnie współpracuje z moim smartfonem). \n
+Warty każdej złotówki. To zdecydowanie nie jest zabawka. Porządnie złożony, świetnie zaprojektowany. Spełnia oczekiwania w 100%, gorąco polecam. \n
+Super sprzęt. Zegarek i do sportu i do noszenia na co dzień. Do tego wykonany z troską o środowisko.</t>
+  </si>
+  <si>
+    <t>Bezprzewodowa łączność ze smartphonem (Android i iOS), automatyczne wykrywanie 3 trybów: bieżnia, bieganie lub spacery na świeżym powietrzu. \n
+Przy standardowym użytkowaniu  do 14 dni na jednym naładowaniu baterii - w trybie oszczędzania baterii maksymalnie do 20 dni. \n
+Ślad węglowy: 36 kg</t>
+  </si>
+  <si>
+    <t>Bardzo dobry zakup. Wygląda jak smartwatch, estetycznie wykonany , posiada wielorakie funkcje, których szukałem. No i możliwości sparowania są na plus! \n
+Udany zakup. Spełnił wszystkie moje oczekiwania. Nawet na chudszej ręce dobrze się prezentuje. Zgrabny, czytelny, wygodny. \n
 Przyjazny środowisku :) . Do tego wygląda jak opaska, ale możliwości ma raczej smartwatcha. Dla mnie super!</t>
-  </si>
-  <si>
-    <t>Ekran o przekątnej 15.6" i wysokiej rozdzielczości z matową powłoką ograniczającą odbijanie się promieni słonecznych\n 
-Dwurdzeniowy procesor i 8 GB pamięci RAM  pozwalającej na uruchomienie kilku aplikacji jednocześnie oraz granie w wymagające sprzętowo gry komputerowe, pojemność dysku SSD 256 GB.\n
-Ślad węglowy to 423 kg</t>
-  </si>
-  <si>
-    <t>png/smartband.png</t>
   </si>
 </sst>
 </file>
@@ -974,8 +974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1007,10 +1007,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
         <v>12</v>
@@ -1024,10 +1024,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s">
         <v>13</v>
@@ -1044,7 +1044,7 @@
         <v>21</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D4" t="s">
         <v>14</v>
@@ -1058,16 +1058,16 @@
         <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D5" t="s">
         <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add: manipulation check. Update: minor fixes.
</commit_message>
<xml_diff>
--- a/materials/conditions.xlsx
+++ b/materials/conditions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mikolaj/Desktop/eyetracker/materials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59534E7F-2ED3-D648-832D-EEBEA76D78E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEB70913-4055-8142-BE7D-1652779EC2FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4420" yWindow="500" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="conditions" sheetId="1" r:id="rId1"/>
@@ -58,18 +58,6 @@
     <t>smartband</t>
   </si>
   <si>
-    <t>cena: 2259 zł</t>
-  </si>
-  <si>
-    <t>cena: 719 zł</t>
-  </si>
-  <si>
-    <t>cena: 1939 zł</t>
-  </si>
-  <si>
-    <t>cena: 249 zł</t>
-  </si>
-  <si>
     <t>png/smartband.png</t>
   </si>
   <si>
@@ -111,6 +99,18 @@
     <t>Czytelny wyświetlacz 1,4 cala, bezprzewodowa łączność ze smartphonem (Android i iOS), asystent zdrowotny z funkcjami pomiaru ciśnienia i EKG, analizą składu ciała, zaawansowaną analiza snu i czujnikami aktywności fizycznej. \n
 Bateria pracuje do 40 godzin, można ją naładować od 0% w 1 godzinę i 48 minut, posiada 16 GB pamięci wewnętrznej. \n
 Ślad węglowy: 43 kg</t>
+  </si>
+  <si>
+    <t>CENA: 1939 zł</t>
+  </si>
+  <si>
+    <t>CENA: 719 zł</t>
+  </si>
+  <si>
+    <t>CENA: 2259 zł</t>
+  </si>
+  <si>
+    <t>CENA: 249 zł</t>
   </si>
 </sst>
 </file>
@@ -974,8 +974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1007,13 +1007,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
         <v>23</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
@@ -1024,13 +1024,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
@@ -1041,13 +1041,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
@@ -1058,16 +1058,16 @@
         <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>